<commit_message>
excel persona names update
</commit_message>
<xml_diff>
--- a/Overview_Personas.xlsx
+++ b/Overview_Personas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannah/Dropbox/Mein Mac (Hannahs-MBP)/Documents/GitHub/Final_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1475F5B9-6D6E-0E42-9884-2AC5442D616F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C34D895F-EAEE-7E47-9421-93AA91747952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="580" windowWidth="28800" windowHeight="16260" xr2:uid="{9864B0CB-F14A-C44F-BD64-38218D1FA3EC}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
   <si>
     <t>marital_status</t>
   </si>
@@ -52,9 +52,6 @@
     <t>young couples/families</t>
   </si>
   <si>
-    <t>highly educated , older couples / small families</t>
-  </si>
-  <si>
     <t>low income, bigger families</t>
   </si>
   <si>
@@ -160,7 +157,25 @@
     <t>couples, medium-high income, no kids, no online, wine</t>
   </si>
   <si>
-    <t>family oriented, highly educated, medium income, wine, online, deals sometimes, teenager, 40s</t>
+    <t>family oriented,  educated, medium income, wine, online, deals sometimes, teenager, 40s</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> educated , older couples / small families</t>
+  </si>
+  <si>
+    <t>Susana</t>
+  </si>
+  <si>
+    <t>Jennifer</t>
+  </si>
+  <si>
+    <t>Karen</t>
+  </si>
+  <si>
+    <t>Richard</t>
+  </si>
+  <si>
+    <t>Michael</t>
   </si>
 </sst>
 </file>
@@ -231,13 +246,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -559,8 +575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84E23F5C-01A5-6F4F-A2BE-6CAF40685C27}">
   <dimension ref="A3:AB8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="AB13" sqref="AB13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -591,88 +607,88 @@
   <sheetData>
     <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="O3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="P3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="R3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="S3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="T3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="U3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="V3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="W3" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="X3" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z3" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB3" s="7" t="s">
         <v>31</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="M3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="N3" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="O3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="P3" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q3" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="R3" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="S3" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="T3" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="U3" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="V3" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="W3" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="X3" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="Y3" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z3" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="AA3" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="AB3" s="6" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.2">
@@ -682,15 +698,17 @@
       <c r="B4" s="3">
         <v>157</v>
       </c>
-      <c r="C4" s="3"/>
+      <c r="C4" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="D4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>35</v>
+        <v>9</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>34</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G4" s="4">
         <v>81000</v>
@@ -753,10 +771,10 @@
         <v>2</v>
       </c>
       <c r="AA4" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AB4" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.2">
@@ -766,12 +784,14 @@
       <c r="B5" s="3">
         <v>532</v>
       </c>
-      <c r="C5" s="3"/>
+      <c r="C5" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="D5" s="3" t="s">
-        <v>5</v>
+        <v>41</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -840,7 +860,7 @@
         <v>3</v>
       </c>
       <c r="AB5" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.2">
@@ -850,6 +870,9 @@
       <c r="B6">
         <v>593</v>
       </c>
+      <c r="C6" t="s">
+        <v>43</v>
+      </c>
       <c r="D6" t="s">
         <v>4</v>
       </c>
@@ -857,7 +880,7 @@
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G6" s="1">
         <v>30000</v>
@@ -923,7 +946,7 @@
         <v>3</v>
       </c>
       <c r="AB6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.2">
@@ -933,9 +956,11 @@
       <c r="B7" s="3">
         <v>428</v>
       </c>
-      <c r="C7" s="3"/>
+      <c r="C7" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="D7" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E7" s="3">
         <v>1</v>
@@ -1007,7 +1032,7 @@
         <v>2</v>
       </c>
       <c r="AB7" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.2">
@@ -1017,11 +1042,14 @@
       <c r="B8">
         <v>500</v>
       </c>
+      <c r="C8" s="6" t="s">
+        <v>44</v>
+      </c>
       <c r="D8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>36</v>
+        <v>5</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>35</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -1087,10 +1115,10 @@
         <v>0</v>
       </c>
       <c r="AA8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AB8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>